<commit_message>
Fixed chemical eq. in D40
</commit_message>
<xml_diff>
--- a/JATP_full_calculation_2023.xlsx
+++ b/JATP_full_calculation_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20402"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akos\0Admin\Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Akos\0Projects\JATP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E587E191-43B6-40FE-B706-41C76E380229}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BB6CA7-9542-4081-822D-F9808DC6F088}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28710" windowHeight="13815" tabRatio="969" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26228" windowHeight="9600" tabRatio="969" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and Assumptions" sheetId="6" r:id="rId1"/>
@@ -232,9 +232,6 @@
   </si>
   <si>
     <t>C3H3O3- + 5[O] + H2O -&gt; 3HCO3- + 2H+</t>
-  </si>
-  <si>
-    <t>C6H31O2 + 46[O] -&gt; 16HCO3- + 15H+</t>
   </si>
   <si>
     <t>20150811 ATP from glycolysis linked to respiration now uses OCRmito not OCRcoupled; Table 1 expanded to include rns and ATP from TCA; ATPoxphos calculated from OCRcoupled for oxphos plus OCRmito for TCA; ranges -&gt;SEM</t>
@@ -643,6 +640,9 @@
   </si>
   <si>
     <t>Cite: Mookerjee SA, Gerencser AA, Nicholls DG, Brand MD. Quantifying intracellular rates of glycolytic and oxidative ATP production and consumption using extracellular flux measurements. Journal of Biological Chemistry. 2017;292(17):7189-207. Epub 20170307. doi: 10.1074/jbc.M116.774471. PubMed PMID: 28270511; PMCID: PMC5409486.</t>
+  </si>
+  <si>
+    <t>C16H31O2 + 46[O] -&gt; 16HCO3- + 15H+</t>
   </si>
 </sst>
 </file>
@@ -7381,7 +7381,7 @@
   <dimension ref="B1:X65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7403,7 +7403,7 @@
         <v>24</v>
       </c>
       <c r="J1" s="130" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -7411,12 +7411,12 @@
         <v>29</v>
       </c>
       <c r="J2" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="2:22" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B3" s="129" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.45">
@@ -7432,7 +7432,7 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
       <c r="K4" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
@@ -7482,7 +7482,7 @@
       <c r="E6" s="23"/>
       <c r="F6" s="23"/>
       <c r="G6" s="142" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
@@ -7515,7 +7515,7 @@
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
       <c r="K7" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L7" s="23"/>
       <c r="M7" s="23"/>
@@ -7534,7 +7534,7 @@
         <v>26</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -7546,7 +7546,7 @@
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
       <c r="K8" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
@@ -7577,7 +7577,7 @@
       <c r="I9" s="23"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
@@ -7593,7 +7593,7 @@
     </row>
     <row r="10" spans="2:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="28"/>
@@ -7635,7 +7635,7 @@
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L12" s="31"/>
       <c r="M12" s="31"/>
@@ -7664,7 +7664,7 @@
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
       <c r="K13" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
@@ -7695,7 +7695,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
@@ -7724,7 +7724,7 @@
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
@@ -7753,7 +7753,7 @@
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
@@ -7782,7 +7782,7 @@
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L17" s="34"/>
       <c r="M17" s="34"/>
@@ -7811,7 +7811,7 @@
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
@@ -7840,7 +7840,7 @@
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
@@ -7869,7 +7869,7 @@
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L20" s="34"/>
       <c r="M20" s="34"/>
@@ -7898,7 +7898,7 @@
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
       <c r="K21" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
@@ -7927,7 +7927,7 @@
       <c r="I22" s="34"/>
       <c r="J22" s="34"/>
       <c r="K22" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L22" s="34"/>
       <c r="M22" s="34"/>
@@ -7971,7 +7971,7 @@
     </row>
     <row r="24" spans="2:22" s="75" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B24" s="103" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" s="89"/>
       <c r="D24" s="89"/>
@@ -7998,7 +7998,7 @@
     </row>
     <row r="25" spans="2:22" s="75" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B25" s="103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" s="89"/>
       <c r="D25" s="89"/>
@@ -8025,7 +8025,7 @@
     </row>
     <row r="26" spans="2:22" s="75" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B26" s="103" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
@@ -8052,7 +8052,7 @@
     </row>
     <row r="27" spans="2:22" s="75" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B27" s="103" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="89"/>
       <c r="D27" s="89"/>
@@ -8167,7 +8167,7 @@
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B31" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="34"/>
       <c r="D31" s="34"/>
@@ -8228,7 +8228,7 @@
     <row r="33" spans="2:24" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="34" spans="2:24" x14ac:dyDescent="0.45">
       <c r="B34" s="42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="43"/>
       <c r="D34" s="43"/>
@@ -8260,26 +8260,26 @@
       <c r="G35" s="47"/>
       <c r="H35" s="47"/>
       <c r="I35" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="J35" s="69" t="s">
         <v>73</v>
-      </c>
-      <c r="J35" s="69" t="s">
-        <v>74</v>
       </c>
       <c r="K35" s="69" t="s">
         <v>61</v>
       </c>
       <c r="L35" s="48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M35" s="69"/>
       <c r="N35" s="69" t="s">
         <v>64</v>
       </c>
       <c r="O35" s="69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P35" s="69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q35" s="69"/>
       <c r="R35" s="57" t="s">
@@ -8298,7 +8298,7 @@
         <v>54</v>
       </c>
       <c r="W35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.45">
@@ -8312,7 +8312,7 @@
       <c r="G36" s="47"/>
       <c r="H36" s="47"/>
       <c r="I36" s="69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J36" s="69" t="s">
         <v>63</v>
@@ -8344,7 +8344,7 @@
       <c r="U36" s="48"/>
       <c r="V36" s="61"/>
       <c r="X36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.45">
@@ -8545,7 +8545,7 @@
       </c>
       <c r="C40" s="46"/>
       <c r="D40" s="47" t="s">
-        <v>70</v>
+        <v>153</v>
       </c>
       <c r="E40" s="47"/>
       <c r="F40" s="47"/>
@@ -8605,7 +8605,7 @@
       </c>
       <c r="C41" s="46"/>
       <c r="D41" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E41" s="47"/>
       <c r="F41" s="47"/>
@@ -8671,7 +8671,7 @@
       </c>
       <c r="C42" s="47"/>
       <c r="D42" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E42" s="47"/>
       <c r="F42" s="47"/>
@@ -8758,7 +8758,7 @@
     </row>
     <row r="44" spans="2:24" x14ac:dyDescent="0.45">
       <c r="B44" s="49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" s="46"/>
       <c r="D44" s="47"/>
@@ -8789,7 +8789,7 @@
       </c>
       <c r="C45" s="46"/>
       <c r="D45" s="47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E45" s="47"/>
       <c r="F45" s="47"/>
@@ -8849,7 +8849,7 @@
       </c>
       <c r="C46" s="47"/>
       <c r="D46" s="47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E46" s="47"/>
       <c r="F46" s="47"/>
@@ -8911,7 +8911,7 @@
       </c>
       <c r="C47" s="51"/>
       <c r="D47" s="51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E47" s="51"/>
       <c r="F47" s="51"/>
@@ -8994,7 +8994,7 @@
     </row>
     <row r="49" spans="2:24" s="87" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B49" s="81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C49" s="82"/>
       <c r="D49" s="82"/>
@@ -9029,15 +9029,15 @@
       <c r="H50" s="89"/>
       <c r="I50" s="90"/>
       <c r="J50" s="91" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K50" s="89"/>
       <c r="L50" s="91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M50" s="89"/>
       <c r="N50" s="89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O50" s="90"/>
       <c r="P50" s="90"/>
@@ -9052,11 +9052,11 @@
     </row>
     <row r="51" spans="2:24" s="87" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B51" s="88" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C51" s="89"/>
       <c r="D51" s="89" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E51" s="89"/>
       <c r="F51" s="89"/>
@@ -9081,11 +9081,11 @@
     </row>
     <row r="52" spans="2:24" s="87" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B52" s="88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C52" s="89"/>
       <c r="D52" s="89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E52" s="89"/>
       <c r="F52" s="89"/>
@@ -9110,11 +9110,11 @@
     </row>
     <row r="53" spans="2:24" s="87" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B53" s="88" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C53" s="89"/>
       <c r="D53" s="89" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E53" s="89"/>
       <c r="F53" s="89"/>
@@ -9141,11 +9141,11 @@
     </row>
     <row r="54" spans="2:24" s="87" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B54" s="88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C54" s="89"/>
       <c r="D54" s="89" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E54" s="89"/>
       <c r="F54" s="89"/>
@@ -9219,47 +9219,47 @@
     </row>
     <row r="57" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="127" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="2:24" x14ac:dyDescent="0.45">
       <c r="B58" s="127" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="2:24" x14ac:dyDescent="0.45">
       <c r="B59" s="127" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="2:24" x14ac:dyDescent="0.45">
       <c r="B60" s="127" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="2:24" x14ac:dyDescent="0.45">
       <c r="B61" s="127" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="2:24" x14ac:dyDescent="0.45">
       <c r="B62" s="127" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="2:24" x14ac:dyDescent="0.45">
       <c r="B63" s="127" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="2:24" s="130" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B64" s="127" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B65" s="127" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -9303,7 +9303,7 @@
     </row>
     <row r="2" spans="1:25" ht="16.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -9346,7 +9346,7 @@
     <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B5" s="123"/>
       <c r="C5" s="155" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5" s="155"/>
       <c r="E5" s="155"/>
@@ -9385,16 +9385,16 @@
         <v>20</v>
       </c>
       <c r="R5" s="146" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S5" s="146"/>
       <c r="T5" s="147" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U5" s="147"/>
       <c r="V5" s="147"/>
       <c r="W5" s="148" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="X5" s="148"/>
       <c r="Y5" s="12"/>
@@ -9402,12 +9402,12 @@
     <row r="6" spans="1:25" ht="43.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="123"/>
       <c r="C6" s="149" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="149"/>
       <c r="E6" s="149"/>
       <c r="F6" s="106" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G6" s="123" t="s">
         <v>10</v>
@@ -9422,10 +9422,10 @@
         <v>15</v>
       </c>
       <c r="K6" s="106" t="s">
+        <v>125</v>
+      </c>
+      <c r="L6" s="123" t="s">
         <v>126</v>
-      </c>
-      <c r="L6" s="123" t="s">
-        <v>127</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>17</v>
@@ -9443,28 +9443,28 @@
         <v>23</v>
       </c>
       <c r="R6" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="S6" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="S6" s="106" t="s">
+      <c r="T6" s="106" t="s">
         <v>118</v>
       </c>
-      <c r="T6" s="106" t="s">
+      <c r="U6" s="106" t="s">
         <v>119</v>
       </c>
-      <c r="U6" s="106" t="s">
+      <c r="V6" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="V6" s="106" t="s">
-        <v>121</v>
-      </c>
       <c r="W6" s="106" t="s">
+        <v>122</v>
+      </c>
+      <c r="X6" s="123" t="s">
         <v>123</v>
       </c>
-      <c r="X6" s="123" t="s">
-        <v>124</v>
-      </c>
       <c r="Y6" s="115" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.45">
@@ -9477,7 +9477,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="150" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I7" s="150"/>
       <c r="J7" s="150"/>
@@ -9534,19 +9534,19 @@
     <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" s="75"/>
       <c r="B9" s="125" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="13">
         <v>0</v>
       </c>
       <c r="E9" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="120" t="s">
         <v>130</v>
-      </c>
-      <c r="F9" s="120" t="s">
-        <v>131</v>
       </c>
       <c r="G9" s="14">
         <v>10</v>
@@ -9623,19 +9623,19 @@
     <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" s="75"/>
       <c r="B10" s="125" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" s="13">
         <v>0</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F10" s="120" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G10" s="14">
         <v>10</v>
@@ -9712,19 +9712,19 @@
     <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11" s="75"/>
       <c r="B11" s="125" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="13">
         <v>0</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F11" s="120" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G11" s="14">
         <v>10</v>
@@ -9857,7 +9857,7 @@
     </row>
     <row r="2" spans="1:25" ht="16.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="132" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="132"/>
       <c r="D2" s="132"/>
@@ -9866,13 +9866,13 @@
     </row>
     <row r="3" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="135" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E3" s="128">
         <v>10000</v>
       </c>
       <c r="F3" s="135" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G3" s="135"/>
     </row>
@@ -9908,7 +9908,7 @@
     <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B5" s="138"/>
       <c r="C5" s="155" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5" s="155"/>
       <c r="E5" s="155"/>
@@ -9947,16 +9947,16 @@
         <v>20</v>
       </c>
       <c r="R5" s="146" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S5" s="146"/>
       <c r="T5" s="147" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U5" s="147"/>
       <c r="V5" s="147"/>
       <c r="W5" s="148" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="X5" s="148"/>
       <c r="Y5" s="12"/>
@@ -9964,12 +9964,12 @@
     <row r="6" spans="1:25" ht="43.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="138"/>
       <c r="C6" s="149" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="149"/>
       <c r="E6" s="149"/>
       <c r="F6" s="126" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G6" s="138" t="s">
         <v>10</v>
@@ -9984,7 +9984,7 @@
         <v>15</v>
       </c>
       <c r="K6" s="126" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L6" s="126" t="str">
         <f>"per "&amp;E3&amp;" cells"</f>
@@ -10006,28 +10006,28 @@
         <v>23</v>
       </c>
       <c r="R6" s="126" t="s">
+        <v>116</v>
+      </c>
+      <c r="S6" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="S6" s="126" t="s">
+      <c r="T6" s="126" t="s">
         <v>118</v>
       </c>
-      <c r="T6" s="126" t="s">
+      <c r="U6" s="126" t="s">
         <v>119</v>
       </c>
-      <c r="U6" s="126" t="s">
+      <c r="V6" s="126" t="s">
         <v>120</v>
       </c>
-      <c r="V6" s="126" t="s">
-        <v>121</v>
-      </c>
       <c r="W6" s="126" t="s">
+        <v>122</v>
+      </c>
+      <c r="X6" s="138" t="s">
         <v>123</v>
       </c>
-      <c r="X6" s="138" t="s">
-        <v>124</v>
-      </c>
       <c r="Y6" s="115" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.45">
@@ -10037,10 +10037,10 @@
       <c r="E7" s="138"/>
       <c r="F7" s="138"/>
       <c r="G7" s="138" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H7" s="150" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I7" s="150"/>
       <c r="J7" s="150"/>
@@ -10100,19 +10100,19 @@
     <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" s="75"/>
       <c r="B9" s="125" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="13">
         <v>0</v>
       </c>
       <c r="E9" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="120" t="s">
         <v>130</v>
-      </c>
-      <c r="F9" s="120" t="s">
-        <v>131</v>
       </c>
       <c r="G9" s="14">
         <v>10000</v>
@@ -10189,19 +10189,19 @@
     <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" s="75"/>
       <c r="B10" s="125" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" s="13">
         <v>0</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F10" s="120" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G10" s="14">
         <v>10000</v>
@@ -10278,19 +10278,19 @@
     <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11" s="75"/>
       <c r="B11" s="125" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="13">
         <v>0</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F11" s="120" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G11" s="14">
         <v>10000</v>
@@ -10366,7 +10366,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="H13" s="130" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>